<commit_message>
Add additional classes + Update HUP Template
</commit_message>
<xml_diff>
--- a/HUP/origineel (niet aanpassen).xlsx
+++ b/HUP/origineel (niet aanpassen).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/twan/Documents/GitHub/VRGZO_HUP_Generator/HUP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED1CA11-A631-2647-A7E2-D8452C2CFC92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ADCC832-BEC5-7C46-B9A2-29CCE83D8FCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Controle objecten" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
   <si>
     <t>Archiefnummer</t>
   </si>
@@ -116,6 +116,15 @@
   </si>
   <si>
     <t>SBI1</t>
+  </si>
+  <si>
+    <t>SBI Omschrijving</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -248,7 +257,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -329,6 +338,7 @@
     <xf numFmtId="164" fontId="11" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Neutraal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1063,10 +1073,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R67"/>
+  <dimension ref="A1:X67"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U6" sqref="U6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1086,10 +1096,12 @@
     <col min="14" max="14" width="57.5" style="13" customWidth="1"/>
     <col min="15" max="15" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="256" width="8.83203125" customWidth="1"/>
+    <col min="17" max="18" width="8.83203125" customWidth="1"/>
+    <col min="19" max="19" width="15.6640625" customWidth="1"/>
+    <col min="20" max="256" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
@@ -1144,8 +1156,20 @@
       <c r="R1" s="10" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="S1" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="T1" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="U1" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="V1" s="23"/>
+      <c r="W1" s="23"/>
+      <c r="X1" s="23"/>
+    </row>
+    <row r="2" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="I2" s="1"/>
       <c r="J2" s="2"/>
       <c r="K2" s="31"/>
@@ -1156,7 +1180,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="20"/>
     </row>
-    <row r="3" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="I3" s="1"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
@@ -1166,7 +1190,7 @@
       <c r="P3" s="2"/>
       <c r="Q3" s="20"/>
     </row>
-    <row r="4" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="I4" s="1"/>
       <c r="J4" s="2"/>
       <c r="K4" s="31"/>
@@ -1176,7 +1200,7 @@
       <c r="P4" s="2"/>
       <c r="Q4" s="20"/>
     </row>
-    <row r="5" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="I5" s="1"/>
       <c r="J5" s="2"/>
       <c r="K5" s="31"/>
@@ -1186,7 +1210,7 @@
       <c r="P5" s="2"/>
       <c r="Q5" s="20"/>
     </row>
-    <row r="6" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="I6" s="1"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
@@ -1197,7 +1221,7 @@
       <c r="P6" s="2"/>
       <c r="Q6" s="20"/>
     </row>
-    <row r="7" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="I7" s="1"/>
       <c r="J7" s="2"/>
       <c r="K7" s="32"/>
@@ -1207,7 +1231,7 @@
       <c r="P7" s="2"/>
       <c r="Q7" s="20"/>
     </row>
-    <row r="8" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="I8" s="1"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
@@ -1218,7 +1242,7 @@
       <c r="P8" s="2"/>
       <c r="Q8" s="20"/>
     </row>
-    <row r="9" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="I9" s="1"/>
       <c r="J9" s="2"/>
       <c r="K9" s="32"/>
@@ -1229,7 +1253,7 @@
       <c r="P9" s="2"/>
       <c r="Q9" s="20"/>
     </row>
-    <row r="10" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="I10" s="1"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
@@ -1239,7 +1263,7 @@
       <c r="P10" s="2"/>
       <c r="Q10" s="20"/>
     </row>
-    <row r="11" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="I11" s="1"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
@@ -1250,7 +1274,7 @@
       <c r="P11" s="2"/>
       <c r="Q11" s="20"/>
     </row>
-    <row r="12" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="I12" s="1"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
@@ -1261,7 +1285,7 @@
       <c r="P12" s="2"/>
       <c r="Q12" s="20"/>
     </row>
-    <row r="13" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="I13" s="1"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
@@ -1272,7 +1296,7 @@
       <c r="P13" s="2"/>
       <c r="Q13" s="20"/>
     </row>
-    <row r="14" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="I14" s="1"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
@@ -1283,7 +1307,7 @@
       <c r="P14" s="2"/>
       <c r="Q14" s="20"/>
     </row>
-    <row r="15" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="I15" s="1"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
@@ -1294,7 +1318,7 @@
       <c r="P15" s="2"/>
       <c r="Q15" s="20"/>
     </row>
-    <row r="16" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="I16" s="1"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
@@ -1303,7 +1327,7 @@
       <c r="N16" s="2"/>
       <c r="Q16" s="20"/>
     </row>
-    <row r="17" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="I17" s="1"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
@@ -1314,7 +1338,7 @@
       <c r="P17" s="2"/>
       <c r="Q17" s="20"/>
     </row>
-    <row r="18" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="I18" s="1"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
@@ -1325,7 +1349,7 @@
       <c r="P18" s="2"/>
       <c r="Q18" s="20"/>
     </row>
-    <row r="19" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1340,7 +1364,7 @@
       <c r="M19" s="2"/>
       <c r="Q19" s="20"/>
     </row>
-    <row r="20" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="17"/>
@@ -1350,7 +1374,7 @@
       <c r="O20" s="26"/>
       <c r="P20" s="20"/>
     </row>
-    <row r="21" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A21" s="23" t="s">
         <v>14</v>
       </c>
@@ -1375,8 +1399,14 @@
       <c r="P21" s="23"/>
       <c r="Q21" s="23"/>
       <c r="R21" s="23"/>
-    </row>
-    <row r="22" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="S21" s="23"/>
+      <c r="T21" s="23"/>
+      <c r="U21" s="23"/>
+      <c r="V21" s="23"/>
+      <c r="W21" s="23"/>
+      <c r="X21" s="23"/>
+    </row>
+    <row r="22" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="D22" s="27"/>
       <c r="E22" s="27"/>
       <c r="J22" s="34"/>
@@ -1385,7 +1415,7 @@
       <c r="M22" s="34"/>
       <c r="N22" s="17"/>
     </row>
-    <row r="23" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="D23" s="27"/>
       <c r="E23" s="27"/>
       <c r="J23" s="35"/>
@@ -1394,7 +1424,7 @@
       <c r="M23" s="35"/>
       <c r="N23" s="28"/>
     </row>
-    <row r="24" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A24" s="23" t="s">
         <v>17</v>
       </c>
@@ -1419,8 +1449,14 @@
       <c r="P24" s="23"/>
       <c r="Q24" s="23"/>
       <c r="R24" s="23"/>
-    </row>
-    <row r="25" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="S24" s="23"/>
+      <c r="T24" s="23"/>
+      <c r="U24" s="23"/>
+      <c r="V24" s="23"/>
+      <c r="W24" s="23"/>
+      <c r="X24" s="23"/>
+    </row>
+    <row r="25" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B25" s="29"/>
       <c r="D25" s="27"/>
       <c r="E25" s="27"/>
@@ -1430,7 +1466,7 @@
       <c r="M25" s="35"/>
       <c r="N25" s="28"/>
     </row>
-    <row r="26" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B26" s="29"/>
       <c r="D26" s="27"/>
       <c r="E26" s="27"/>
@@ -1440,7 +1476,7 @@
       <c r="M26" s="35"/>
       <c r="N26" s="28"/>
     </row>
-    <row r="27" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A27" s="23" t="s">
         <v>19</v>
       </c>
@@ -1465,8 +1501,14 @@
       <c r="P27" s="23"/>
       <c r="Q27" s="23"/>
       <c r="R27" s="23"/>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S27" s="23"/>
+      <c r="T27" s="23"/>
+      <c r="U27" s="23"/>
+      <c r="V27" s="23"/>
+      <c r="W27" s="23"/>
+      <c r="X27" s="23"/>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.15">
       <c r="B28" s="29"/>
       <c r="F28" s="8"/>
       <c r="J28" s="35"/>
@@ -1475,7 +1517,7 @@
       <c r="M28" s="36"/>
       <c r="Q28" s="8"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.15">
       <c r="B29" s="29"/>
       <c r="F29" s="8"/>
       <c r="J29" s="35"/>
@@ -1484,7 +1526,7 @@
       <c r="M29" s="36"/>
       <c r="Q29" s="8"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.15">
       <c r="B30" s="29"/>
       <c r="F30" s="8"/>
       <c r="J30" s="35"/>
@@ -1493,7 +1535,7 @@
       <c r="M30" s="36"/>
       <c r="Q30" s="8"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.15">
       <c r="B31" s="29"/>
       <c r="F31" s="8"/>
       <c r="J31" s="35"/>
@@ -1502,7 +1544,7 @@
       <c r="M31" s="36"/>
       <c r="Q31" s="8"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.15">
       <c r="B32" s="29"/>
       <c r="F32" s="8"/>
       <c r="J32" s="35"/>
@@ -1727,7 +1769,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Additional columns and new template
</commit_message>
<xml_diff>
--- a/HUP/origineel (niet aanpassen).xlsx
+++ b/HUP/origineel (niet aanpassen).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/twan/Documents/GitHub/VRGZO_HUP_Generator/HUP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ADCC832-BEC5-7C46-B9A2-29CCE83D8FCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC9A1A66-2246-2D45-96CA-1C05A89716A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
   <si>
     <t>Archiefnummer</t>
   </si>
@@ -125,6 +125,12 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>Bouwjaar</t>
+  </si>
+  <si>
+    <t>Bouwlagen</t>
   </si>
 </sst>
 </file>
@@ -1076,7 +1082,7 @@
   <dimension ref="A1:X67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U6" sqref="U6"/>
+      <selection activeCell="V15" sqref="V15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1098,7 +1104,9 @@
     <col min="16" max="16" width="19.5" bestFit="1" customWidth="1"/>
     <col min="17" max="18" width="8.83203125" customWidth="1"/>
     <col min="19" max="19" width="15.6640625" customWidth="1"/>
-    <col min="20" max="256" width="8.83203125" customWidth="1"/>
+    <col min="20" max="22" width="8.83203125" customWidth="1"/>
+    <col min="23" max="23" width="10.33203125" customWidth="1"/>
+    <col min="24" max="256" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.15">
@@ -1165,8 +1173,12 @@
       <c r="U1" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="V1" s="23"/>
-      <c r="W1" s="23"/>
+      <c r="V1" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="W1" s="23" t="s">
+        <v>29</v>
+      </c>
       <c r="X1" s="23"/>
     </row>
     <row r="2" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.15">

</xml_diff>